<commit_message>
Unddated code and headders in inputs
</commit_message>
<xml_diff>
--- a/clean_data_pythonic.xlsx
+++ b/clean_data_pythonic.xlsx
@@ -436,258 +436,258 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Price Per Unit</t>
+          <t>Price Per Unit (£s)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1054</v>
+        <v>1054.63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1629</v>
+        <v>1629.57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1606</v>
+        <v>1606.67</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1201</v>
+        <v>1201.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1434</v>
+        <v>1434.28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>289</v>
+        <v>289.95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>500</v>
+        <v>500.08</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2100</v>
+        <v>2100.87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>132</v>
+        <v>132.42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>994</v>
+        <v>994.4299999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>896</v>
+        <v>896.17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>905</v>
+        <v>905.11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1076</v>
+        <v>1076.55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1592</v>
+        <v>1592.19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>325</v>
+        <v>325.24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1058</v>
+        <v>1058.77</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>291</v>
+        <v>291.21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1255</v>
+        <v>1255.21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2135</v>
+        <v>2135.78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>497</v>
+        <v>497.25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1129</v>
+        <v>1129.05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>854</v>
+        <v>854.6900000000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>830</v>
+        <v>830.78</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1131</v>
+        <v>1131.27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2449</v>
+        <v>2449.87</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1578</v>
+        <v>1578.02</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2297</v>
+        <v>2297.42</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2606</v>
+        <v>2606.77</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>277</v>
+        <v>277.81</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2172</v>
+        <v>2172.67</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2072</v>
+        <v>2072.84</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>888</v>
+        <v>888.53</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>618</v>
+        <v>618.09</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>644</v>
+        <v>644.99</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2075</v>
+        <v>2075.84</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2581</v>
+        <v>2581.93</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>724</v>
+        <v>724.99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>276</v>
+        <v>276.75</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1432</v>
+        <v>1432.77</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>734</v>
+        <v>734.76</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>39</v>
+        <v>39.34</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2900</v>
+        <v>2900.69</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1199</v>
+        <v>1199.25</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>847</v>
+        <v>847.83</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>650</v>
+        <v>650.3099999999999</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1495</v>
+        <v>1495.55</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2106</v>
+        <v>2106.64</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2213</v>
+        <v>2213.31</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1038</v>
+        <v>1038.88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1595</v>
+        <v>1595.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>